<commit_message>
Reorganised outputs, added scenario runner and inventory simulation, improved plot outputs
</commit_message>
<xml_diff>
--- a/data/timber_ar_estimates.xlsx
+++ b/data/timber_ar_estimates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexSharples\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alex\projects\harvest-timing\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8BE0B71-13B1-4003-906C-B0BC53CE668B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26AF7690-5D8C-4706-905D-AF4CCBF4EB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,20 @@
     <sheet name="Regression" sheetId="2" r:id="rId2"/>
     <sheet name="Estimates" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -856,7 +868,1032 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AllGradesAvg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$A$2:$A$120</c:f>
+              <c:strCache>
+                <c:ptCount val="119"/>
+                <c:pt idx="0">
+                  <c:v>1996-03-01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1996-06-01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1996-09-01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1996-12-01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1997-03-01</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1997-06-01</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1997-09-01</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1997-12-01</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1998-03-01</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1998-06-01</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1998-09-01</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1998-12-01</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1999-03-01</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1999-06-01</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1999-09-01</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1999-12-01</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2000-03-01</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2000-06-01</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2000-09-01</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000-12-01</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2001-03-01</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2001-06-01</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2001-09-01</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2001-12-01</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2002-03-01</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2002-06-01</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2002-09-01</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2002-12-01</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2003-03-01</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2003-06-01</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2003-09-01</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2003-12-01</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2004-03-01</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2004-06-01</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2004-09-01</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2004-12-01</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2005-03-01</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2005-06-01</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2005-09-01</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2005-12-01</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2006-03-01</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2006-06-01</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2006-09-01</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2006-12-01</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2007-03-01</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2007-06-01</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2007-09-01</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2007-12-01</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2008-03-01</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2008-06-01</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2008-09-01</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2008-12-01</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2009-03-01</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2009-06-01</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2009-09-01</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2009-12-01</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2010-03-01</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2010-06-01</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2010-09-01</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2010-12-01</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2011-03-01</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2011-06-01</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2011-09-01</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2011-12-01</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2012-03-01</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2012-06-01</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2012-09-01</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2012-12-01</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2013-03-01</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2013-06-01</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2013-09-01</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2013-12-01</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2014-03-01</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2014-06-01</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2014-09-01</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2014-12-01</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2015-03-01</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2015-06-01</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2015-09-01</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2015-12-01</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2016-03-01</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2016-06-01</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2016-09-01</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2016-12-01</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2017-03-01</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2017-06-01</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2017-09-01</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2017-12-01</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2018-03-01</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2018-06-01</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2018-09-01</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2018-12-01</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2019-03-01</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2019-06-01</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2019-09-01</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2019-12-01</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2020-03-01</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2020-06-01</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2020-09-01</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2020-12-01</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2021-03-01</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2021-06-30</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2021-09-30</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>2021-12-31</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2022-03-31</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>2022-06-30</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>2022-09-30</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>2022-12-31</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>2023-03-31</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>2023-06-30</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>2023-09-30</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>2023-12-31</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>2024-03-31</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>2024-06-30</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>2024-09-30</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>2024-12-31</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>2025-03-31</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>2025-06-30</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>2025-09-30</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$B$2:$B$120</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="119"/>
+                <c:pt idx="0">
+                  <c:v>122.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>113.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>111.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>102.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>110.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>121.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>114.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>108.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>104.4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>101.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>101.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>109.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>111.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>116.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>118.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>121.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>116.1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>107.8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>108.4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>114.2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>121.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>116.4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>118.9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>103.1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>100.4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>95.8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>87.2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>96.8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>88.6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>87.2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>92.4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>93.3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>93.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>88.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>112.1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>116.2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>101.1</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>84.3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>92.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>89.6</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>100.625</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>132.25</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>119.125</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>102.875</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>102.5</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>102.625</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>137.375</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>130.125</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>135.625</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>149.5</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>146.625</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>129.75</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>120.25</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>114.25</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>120.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>122.125</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>119.25</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>135.375</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>144.875</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>153.75</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>156.5</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>154.125</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>132.375</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>127.25</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>146.75</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>122.6346650029687</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>148.125</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>164.5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>152.125</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>160.75</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>166.17928683230289</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>181.91792991670351</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>164.1884141781577</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>128.71636352051431</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>155.2900774233112</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>145.0223728885129</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>147.50291083364439</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>149.4013855486298</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>163.43378033581399</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>131.15567121282879</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>135.8088688891936</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>154.99292788859159</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>151.38330527827799</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>135.46607012513999</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>135.12675023820651</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>152.83146366496189</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>154.29035654219419</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>132.83714207215729</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>132.1763007902305</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5155-468F-9D49-1E91E4FEAF13}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="22210047"/>
+        <c:axId val="22210527"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="22210047"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="22210527"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="22210527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="22210047"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1412,6 +2449,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1445,6 +2998,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDFB4981-F7DF-DE71-BDFE-07B8335FBC77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1740,8 +3329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="V96" sqref="V96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>